<commit_message>
Add dos icones help e modificação inicial do analytics
</commit_message>
<xml_diff>
--- a/documents/xlsx/quartis.xlsx
+++ b/documents/xlsx/quartis.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakar\Desktop\BandTec\Primeiro semestre\Iniciativa 0\startech\documents\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINDOWS10\Desktop\BandTec\Pesquisa e Inovação\Projeto\NoIgnite\documents\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374807F5-13A3-41C7-A2E4-9D4D32A12F3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="28800" windowHeight="11730"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Ideal</t>
   </si>
@@ -72,12 +73,45 @@
   </si>
   <si>
     <t>Alerta 2 Umidade</t>
+  </si>
+  <si>
+    <t>Analytics Conjunta</t>
+  </si>
+  <si>
+    <t>a partir de 35ºC          35%</t>
+  </si>
+  <si>
+    <t>ideal</t>
+  </si>
+  <si>
+    <t>Alerta 1</t>
+  </si>
+  <si>
+    <t>Alerta crítico</t>
+  </si>
+  <si>
+    <t>a partir de 45ºC e menor que 25%</t>
+  </si>
+  <si>
+    <t>*Caso algum parâmetro seja atingido, o alerta será emitido, idependente se o outro parâmetro atingiu ou não</t>
+  </si>
+  <si>
+    <t>Pouco Risco</t>
+  </si>
+  <si>
+    <t>entre 30ºC-35ºC e 50%</t>
+  </si>
+  <si>
+    <t>até 25ºC e a partir 80%</t>
+  </si>
+  <si>
+    <t>entre 25ºC-30º e 60%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -197,11 +231,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,6 +313,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,22 +611,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D13" sqref="D13:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
@@ -546,7 +637,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
@@ -563,7 +654,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -580,7 +671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>7</v>
       </c>
@@ -589,7 +680,7 @@
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
         <v>0</v>
       </c>
@@ -606,7 +697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -623,15 +714,92 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="J19" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="9">
+    <mergeCell ref="B17:I17"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>